<commit_message>
More changes to CRTT coding and script.
</commit_message>
<xml_diff>
--- a/CRTT.xlsx
+++ b/CRTT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="124">
   <si>
     <t>Study</t>
   </si>
@@ -96,15 +96,9 @@
     <t>Brusa, J. A. (1987). Effects of video game playing on children's social behavior. Dissertation: De Paul University, Chicago, IL.</t>
   </si>
   <si>
-    <t>BA02ABF</t>
-  </si>
-  <si>
     <t>Bartholow, B. D., &amp; Anderson, C. A.  (2002). Effects of Violent Video Games on Aggressive Behavior: Potential Sex Differences. Journal of Experimental Social Psychology, 38, 283-290.</t>
   </si>
   <si>
-    <t>BA02ABM</t>
-  </si>
-  <si>
     <t>BBR09AB</t>
   </si>
   <si>
@@ -391,19 +385,28 @@
   </si>
   <si>
     <t>Study.name</t>
+  </si>
+  <si>
+    <t>BA02ABF/BA02ABM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -426,9 +429,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,20 +734,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -752,13 +756,13 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -789,13 +793,13 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,13 +816,13 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -835,13 +839,13 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -858,10 +862,10 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
         <v>91</v>
-      </c>
-      <c r="F6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -878,10 +882,10 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -901,7 +905,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -921,7 +925,7 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -938,13 +942,13 @@
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -961,10 +965,10 @@
         <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -982,32 +986,29 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
       <c r="C14">
         <v>1</v>
       </c>
@@ -1015,10 +1016,10 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="F14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1032,13 +1033,13 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1055,10 +1056,10 @@
         <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1066,7 +1067,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1075,30 +1076,33 @@
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="F18" t="s">
-        <v>105</v>
+        <v>108</v>
+      </c>
+      <c r="G18" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1109,18 +1113,15 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1137,12 +1138,6 @@
       <c r="D20" t="s">
         <v>23</v>
       </c>
-      <c r="E20" t="s">
-        <v>104</v>
-      </c>
-      <c r="F20" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1152,10 +1147,16 @@
         <v>41</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1166,23 +1167,23 @@
         <v>43</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C23">
@@ -1192,10 +1193,10 @@
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="F23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1206,13 +1207,13 @@
         <v>47</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="F24" t="s">
         <v>114</v>
@@ -1222,20 +1223,20 @@
       <c r="A25" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>49</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1249,13 +1250,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" t="s">
-        <v>104</v>
-      </c>
-      <c r="F26" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1283,7 +1278,13 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1297,13 +1298,13 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E29" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="F29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1311,7 +1312,7 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1320,44 +1321,44 @@
         <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" t="s">
-        <v>104</v>
-      </c>
-      <c r="F31" t="s">
-        <v>118</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>62</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="E32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1374,10 +1375,10 @@
         <v>23</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1391,67 +1392,61 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" t="s">
-        <v>121</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>70</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>71</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" t="s">
-        <v>104</v>
-      </c>
-      <c r="F37" t="s">
-        <v>122</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1459,10 +1454,10 @@
         <v>73</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" t="s">
         <v>20</v>
@@ -1470,16 +1465,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="C39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1493,10 +1491,7 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1512,6 +1507,9 @@
       <c r="D41" t="s">
         <v>23</v>
       </c>
+      <c r="E41" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1524,10 +1522,7 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E42" t="s">
-        <v>104</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1543,29 +1538,29 @@
       <c r="D43" t="s">
         <v>4</v>
       </c>
+      <c r="E43" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>87</v>
       </c>
       <c r="C45">
@@ -1575,22 +1570,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>